<commit_message>
Pushed  - 2 on 20/Oct/2019 - Rajkumar from Home
Signed-off-by: Rajkumar <raj4learn@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/CompareQuiresList.xlsx
+++ b/CompareQuiresList.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\CompareMigData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB6F858-0BD5-48C1-8BAD-DBBB94A0861E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A54791-EFBF-4882-9F0B-63D2B7FDD12E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="10890" xr2:uid="{3F338244-30EA-463E-A82E-5FB641311133}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{3F338244-30EA-463E-A82E-5FB641311133}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="2" r:id="rId1"/>
     <sheet name="TableList" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Bkp" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="28">
   <si>
     <t>Source_Tabel</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>PROCESS_FLAG</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>TABLE_NAME</t>
@@ -482,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0139B1F6-6BDB-499E-B3C3-74F67D5C3F01}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +499,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -510,58 +507,58 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -574,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56FA3C68-F1F1-4F32-A5C5-56BFD5092EF3}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A6:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +607,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -619,7 +616,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -630,13 +627,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -644,13 +641,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -658,13 +655,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -672,19 +669,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -692,19 +689,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
@@ -712,47 +709,47 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
         <v>6</v>
@@ -760,61 +757,61 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
@@ -822,16 +819,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -845,7 +842,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F15"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,7 +869,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -881,7 +878,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -892,13 +889,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -906,13 +903,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -920,13 +917,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -934,19 +931,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -954,19 +951,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
@@ -974,47 +971,47 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
         <v>6</v>
@@ -1022,61 +1019,61 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
@@ -1084,16 +1081,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>